<commit_message>
added mp4 files, added a How To page.
</commit_message>
<xml_diff>
--- a/data_intermediate/diseasetrait_naming_conversion.xlsx
+++ b/data_intermediate/diseasetrait_naming_conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karinemoussa/Documents/DrLiu_Lab/Shiny_Apps/xci-app-1/data_intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83249736-209A-6E46-AF6F-172706744DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054D3B77-0F37-DA43-BE6C-5DB9ECDAF0F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-200" yWindow="-19900" windowWidth="31680" windowHeight="15860" xr2:uid="{CD089294-1F05-E948-8928-BB4B549864DB}"/>
+    <workbookView xWindow="-200" yWindow="-19900" windowWidth="31680" windowHeight="15860" activeTab="1" xr2:uid="{CD089294-1F05-E948-8928-BB4B549864DB}"/>
   </bookViews>
   <sheets>
     <sheet name="UKBIO_list" sheetId="1" r:id="rId1"/>
@@ -9765,7 +9765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9412DD1-8B46-F046-8E59-DD463C0416FE}">
   <dimension ref="A1:D320"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
@@ -11551,12 +11551,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAB156A-F1D2-EC44-883B-91991D29CBD6}">
   <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I262" sqref="I262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="62.83203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
continuing to work through disease trait conversion list. ref #33
</commit_message>
<xml_diff>
--- a/data_intermediate/diseasetrait_naming_conversion.xlsx
+++ b/data_intermediate/diseasetrait_naming_conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karinemoussa/Documents/DrLiu_Lab/Shiny_Apps/xci-app-1/data_intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054D3B77-0F37-DA43-BE6C-5DB9ECDAF0F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD4D9B2-C6F7-8644-B133-E85411474913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-200" yWindow="-19900" windowWidth="31680" windowHeight="15860" activeTab="1" xr2:uid="{CD089294-1F05-E948-8928-BB4B549864DB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{CD089294-1F05-E948-8928-BB4B549864DB}"/>
   </bookViews>
   <sheets>
     <sheet name="UKBIO_list" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3656" uniqueCount="3111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3679" uniqueCount="3112">
   <si>
     <t>DISEASE/TRAIT</t>
   </si>
@@ -9375,6 +9375,9 @@
   </si>
   <si>
     <t>Alcohol dependence, Depression and alcohol dependence</t>
+  </si>
+  <si>
+    <t>alopecia, alopecia areata</t>
   </si>
 </sst>
 </file>
@@ -9765,8 +9768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9412DD1-8B46-F046-8E59-DD463C0416FE}">
   <dimension ref="A1:D320"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A275" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C285" sqref="C285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9851,51 +9854,95 @@
       <c r="A8" t="s">
         <v>2930</v>
       </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2929</v>
       </c>
+      <c r="B9" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3099</v>
       </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2924</v>
       </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3098</v>
       </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="s">
+        <v>3111</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>3111</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2964</v>
       </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2998</v>
       </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2812</v>
       </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2907</v>
       </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2980</v>
       </c>
+      <c r="B17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -11264,82 +11311,91 @@
         <v>3091</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>3044</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>2927</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>2831</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>2878</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>2887</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>3019</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>2905</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>2833</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>2835</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>3058</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>2821</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>2820</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>2990</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>2926</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B287" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C287" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D287" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>3061</v>
       </c>
@@ -11551,8 +11607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAB156A-F1D2-EC44-883B-91991D29CBD6}">
   <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I262" sqref="I262"/>
+    <sheetView topLeftCell="A225" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B238" sqref="B238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11643,6 +11699,9 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>2980</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>93</v>
       </c>
@@ -11919,6 +11978,9 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>2929</v>
+      </c>
       <c r="B70" s="1" t="s">
         <v>189</v>
       </c>
@@ -12723,82 +12785,85 @@
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B225" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B226" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B227" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B228" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B229" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B230" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B231" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B232" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B233" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B234" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B235" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B236" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B237" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>2926</v>
+      </c>
       <c r="B238" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B239" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B240" s="1" t="s">
         <v>208</v>
       </c>
@@ -12999,12 +13064,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC87240-39B2-2D45-960E-6784B043F1CF}">
   <dimension ref="A1:B436"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+    <sheetView topLeftCell="A248" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="55.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13090,86 +13156,92 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>3098</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>3098</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>568</v>
       </c>
@@ -14333,6 +14405,9 @@
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>2926</v>
+      </c>
       <c r="B261" s="1" t="s">
         <v>294</v>
       </c>
@@ -14967,82 +15042,85 @@
         <v>694</v>
       </c>
     </row>
-    <row r="385" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B385" s="1" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="386" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B386" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="387" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B387" s="1" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="388" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B388" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="389" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A389" t="s">
+        <v>2907</v>
+      </c>
       <c r="B389" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="390" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B390" s="1" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="391" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B391" s="1" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="392" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B392" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="393" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B393" s="1" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="394" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B394" s="1" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="395" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B395" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="396" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B396" s="1" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="397" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B397" s="1" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="398" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B398" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="399" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B399" s="1" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="400" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B400" s="1" t="s">
         <v>701</v>
       </c>
@@ -15240,8 +15318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A27DD5-9C45-4540-ACA5-15A282443161}">
   <dimension ref="A1:B2533"/>
   <sheetViews>
-    <sheetView topLeftCell="A1119" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A1133" sqref="A1133"/>
+    <sheetView topLeftCell="A1476" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1489" sqref="B1489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15656,82 +15734,88 @@
         <v>900</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B81" s="1" t="s">
         <v>901</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>3098</v>
+      </c>
       <c r="B83" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>3098</v>
+      </c>
       <c r="B84" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="s">
         <v>902</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="s">
         <v>903</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
         <v>1719</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B88" s="1" t="s">
         <v>2175</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B89" s="1" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B91" s="1" t="s">
         <v>1990</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B92" s="1" t="s">
         <v>2692</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" s="1" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B94" s="1" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B95" s="1" t="s">
         <v>910</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B96" s="1" t="s">
         <v>911</v>
       </c>
@@ -15976,82 +16060,85 @@
         <v>947</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B145" s="1" t="s">
         <v>949</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B146" s="1" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B147" s="1" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B148" s="1" t="s">
         <v>1639</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B149" s="1" t="s">
         <v>1145</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B150" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B151" s="1" t="s">
         <v>951</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>2980</v>
+      </c>
       <c r="B152" s="1" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B153" s="1" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B154" s="1" t="s">
         <v>904</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B155" s="1" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B156" s="1" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B157" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B158" s="1" t="s">
         <v>2700</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B159" s="1" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B160" s="1" t="s">
         <v>468</v>
       </c>
@@ -16859,82 +16946,85 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="321" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B321" s="1" t="s">
         <v>885</v>
       </c>
     </row>
-    <row r="322" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B322" s="1" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="323" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B323" s="1" t="s">
         <v>1599</v>
       </c>
     </row>
-    <row r="324" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B324" s="1" t="s">
         <v>2616</v>
       </c>
     </row>
-    <row r="325" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
+        <v>2980</v>
+      </c>
       <c r="B325" s="1" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B326" s="1" t="s">
         <v>1068</v>
       </c>
     </row>
-    <row r="327" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B327" s="1" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="328" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B328" s="1" t="s">
         <v>2302</v>
       </c>
     </row>
-    <row r="329" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B329" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="330" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B330" s="1" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="331" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B331" s="1" t="s">
         <v>1160</v>
       </c>
     </row>
-    <row r="332" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B332" s="1" t="s">
         <v>1073</v>
       </c>
     </row>
-    <row r="333" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B333" s="1" t="s">
         <v>1074</v>
       </c>
     </row>
-    <row r="334" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B334" s="1" t="s">
         <v>1076</v>
       </c>
     </row>
-    <row r="335" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B335" s="1" t="s">
         <v>1077</v>
       </c>
     </row>
-    <row r="336" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B336" s="1" t="s">
         <v>1078</v>
       </c>
@@ -22714,82 +22804,85 @@
         <v>432</v>
       </c>
     </row>
-    <row r="1489" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1489" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1489" t="s">
+        <v>2926</v>
+      </c>
       <c r="B1489" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="1490" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1490" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1490" s="1" t="s">
         <v>1966</v>
       </c>
     </row>
-    <row r="1491" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1491" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1491" s="1" t="s">
         <v>1967</v>
       </c>
     </row>
-    <row r="1492" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1492" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1492" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="1493" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1493" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1493" s="1" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="1494" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1494" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1494" s="1" t="s">
         <v>1968</v>
       </c>
     </row>
-    <row r="1495" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1495" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1495" s="1" t="s">
         <v>1970</v>
       </c>
     </row>
-    <row r="1496" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1496" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1496" s="1" t="s">
         <v>1969</v>
       </c>
     </row>
-    <row r="1497" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1497" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1497" s="1" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="1498" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1498" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1498" s="1" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="1499" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1499" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1499" s="1" t="s">
         <v>1971</v>
       </c>
     </row>
-    <row r="1500" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1500" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1500" s="1" t="s">
         <v>2794</v>
       </c>
     </row>
-    <row r="1501" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1501" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1501" s="1" t="s">
         <v>1973</v>
       </c>
     </row>
-    <row r="1502" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1502" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1502" s="1" t="s">
         <v>1975</v>
       </c>
     </row>
-    <row r="1503" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1503" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1503" s="1" t="s">
         <v>1974</v>
       </c>
     </row>
-    <row r="1504" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1504" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1504" s="1" t="s">
         <v>1977</v>
       </c>
@@ -26732,82 +26825,85 @@
         <v>2630</v>
       </c>
     </row>
-    <row r="2289" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2289" s="1" t="s">
         <v>2631</v>
       </c>
     </row>
-    <row r="2290" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2290" s="1" t="s">
         <v>2632</v>
       </c>
     </row>
-    <row r="2291" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2291" s="1" t="s">
         <v>2633</v>
       </c>
     </row>
-    <row r="2292" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2292" s="1" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="2293" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2293" s="1" t="s">
         <v>2635</v>
       </c>
     </row>
-    <row r="2294" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2294" s="1" t="s">
         <v>978</v>
       </c>
     </row>
-    <row r="2295" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2295" s="1" t="s">
         <v>2636</v>
       </c>
     </row>
-    <row r="2296" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2296" s="1" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="2297" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2297" s="1" t="s">
         <v>1265</v>
       </c>
     </row>
-    <row r="2298" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2298" s="1" t="s">
         <v>2638</v>
       </c>
     </row>
-    <row r="2299" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2299" s="1" t="s">
         <v>2639</v>
       </c>
     </row>
-    <row r="2300" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2300" s="1" t="s">
         <v>1994</v>
       </c>
     </row>
-    <row r="2301" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2301" s="1" t="s">
         <v>2640</v>
       </c>
     </row>
-    <row r="2302" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2302" s="1" t="s">
         <v>2641</v>
       </c>
     </row>
-    <row r="2303" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2303" t="s">
+        <v>2907</v>
+      </c>
       <c r="B2303" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="2304" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2304" s="1" t="s">
         <v>2642</v>
       </c>

</xml_diff>

<commit_message>
finished conversion chart, added sex bias information to search. Closes #33
</commit_message>
<xml_diff>
--- a/data_intermediate/diseasetrait_naming_conversion.xlsx
+++ b/data_intermediate/diseasetrait_naming_conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karinemoussa/Documents/DrLiu_Lab/Shiny_Apps/xci-app-1/data_intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C330967-2715-3746-8B0E-E72029B7D540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574201DC-CAA1-F94D-8150-40449164EA7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{CD089294-1F05-E948-8928-BB4B549864DB}"/>
+    <workbookView xWindow="180" yWindow="560" windowWidth="28800" windowHeight="16100" xr2:uid="{CD089294-1F05-E948-8928-BB4B549864DB}"/>
   </bookViews>
   <sheets>
     <sheet name="UKBIO_list" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4150" uniqueCount="3138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4361" uniqueCount="3149">
   <si>
     <t>DISEASE/TRAIT</t>
   </si>
@@ -9434,9 +9434,6 @@
     <t>iron deficiency anemia; iron-refractory iron deficiency anemia</t>
   </si>
   <si>
-    <t>nephrolithiasis; nephrolithiasis, x-linked recessive, with renal failure</t>
-  </si>
-  <si>
     <t>cirrhosis, familial; north american indian childhood cirrhosis</t>
   </si>
   <si>
@@ -9456,6 +9453,42 @@
   </si>
   <si>
     <t>osteoporosis; osteoporosis-pseudoglioma syndrome</t>
+  </si>
+  <si>
+    <t>polycystic kidney; polycystic kidney, autosomal recessive</t>
+  </si>
+  <si>
+    <t>retinal diseases; retinal vasculitis</t>
+  </si>
+  <si>
+    <t>************</t>
+  </si>
+  <si>
+    <t>rheumatoid arthritis; Rheumatoid arthritis (ACPA-positive)</t>
+  </si>
+  <si>
+    <t>sarcoidosis; sarcoidosis, early-onset</t>
+  </si>
+  <si>
+    <t>testicular microlithiasis; testicular neoplasms</t>
+  </si>
+  <si>
+    <t>alpha-thalassemia; alpha-thalassemia myelodysplasia syndrome; beta-thalassemia</t>
+  </si>
+  <si>
+    <t>thyroid diseases; thyroid hormones</t>
+  </si>
+  <si>
+    <t>*************</t>
+  </si>
+  <si>
+    <t>Tuberculosis; Tuberculosis (SNP x SNP interaction)</t>
+  </si>
+  <si>
+    <t>nephrolithiasis; urinary calculi; kidney calculi</t>
+  </si>
+  <si>
+    <t>nephrolithiasis; nephrolithiasis, x-linked recessive, with renal failure; urinary calculi; kidney calculi</t>
   </si>
 </sst>
 </file>
@@ -9494,7 +9527,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9513,6 +9546,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -9526,7 +9565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -9538,6 +9577,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9854,8 +9894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9412DD1-8B46-F046-8E59-DD463C0416FE}">
   <dimension ref="A1:H320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="144" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B246" sqref="B246"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E317" sqref="E317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11758,10 +11798,10 @@
       </c>
       <c r="B173" s="4"/>
       <c r="C173" s="5" t="s">
-        <v>279</v>
+        <v>3147</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>3130</v>
+        <v>3148</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>1848</v>
@@ -11809,7 +11849,7 @@
       <c r="B178" s="4"/>
       <c r="C178" s="5"/>
       <c r="D178" s="5" t="s">
-        <v>3131</v>
+        <v>3130</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -11850,11 +11890,11 @@
       </c>
       <c r="B182" s="4"/>
       <c r="C182" s="4" t="s">
-        <v>3133</v>
+        <v>3132</v>
       </c>
       <c r="D182" s="4"/>
       <c r="F182" t="s">
-        <v>3134</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
@@ -12063,7 +12103,7 @@
       <c r="C199" s="4"/>
       <c r="D199" s="4"/>
       <c r="F199" t="s">
-        <v>3135</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
@@ -12073,7 +12113,7 @@
       <c r="B200" s="4"/>
       <c r="C200" s="4"/>
       <c r="D200" s="4" t="s">
-        <v>3135</v>
+        <v>3134</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>1018</v>
@@ -12118,10 +12158,10 @@
       </c>
       <c r="B204" s="4"/>
       <c r="C204" s="5" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>2111</v>
@@ -12228,7 +12268,7 @@
         <v>561</v>
       </c>
       <c r="D213" s="5" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>2179</v>
@@ -12238,7 +12278,9 @@
       <c r="A214" t="s">
         <v>2837</v>
       </c>
-      <c r="D214" s="1"/>
+      <c r="B214" s="4"/>
+      <c r="C214" s="4"/>
+      <c r="D214" s="5"/>
       <c r="F214" s="1" t="s">
         <v>2180</v>
       </c>
@@ -12262,16 +12304,29 @@
       <c r="A216" t="s">
         <v>2955</v>
       </c>
+      <c r="B216" s="4"/>
+      <c r="C216" s="4"/>
+      <c r="D216" s="4"/>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>2937</v>
       </c>
+      <c r="B217" s="4"/>
+      <c r="C217" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="D217" s="5" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>2829</v>
       </c>
+      <c r="B218" s="4"/>
+      <c r="C218" s="4"/>
+      <c r="D218" s="4"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
@@ -12395,16 +12450,29 @@
       <c r="A233" t="s">
         <v>2871</v>
       </c>
+      <c r="B233" s="4"/>
+      <c r="C233" s="5" t="s">
+        <v>2369</v>
+      </c>
+      <c r="D233" s="5" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>3022</v>
       </c>
+      <c r="B234" s="4"/>
+      <c r="C234" s="4"/>
+      <c r="D234" s="4"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>2832</v>
       </c>
+      <c r="B235" s="4"/>
+      <c r="C235" s="4"/>
+      <c r="D235" s="4"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
@@ -12420,31 +12488,57 @@
       <c r="A237" t="s">
         <v>2994</v>
       </c>
+      <c r="B237" s="4"/>
+      <c r="C237" s="4"/>
+      <c r="D237" s="5"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>3012</v>
       </c>
+      <c r="B238" s="4"/>
+      <c r="C238" s="4"/>
+      <c r="D238" s="4"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>2951</v>
       </c>
+      <c r="B239" s="4"/>
+      <c r="C239" s="4"/>
+      <c r="D239" s="4" t="s">
+        <v>3137</v>
+      </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>2915</v>
       </c>
+      <c r="B240" s="4"/>
+      <c r="C240" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="D240" s="5" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>2959</v>
       </c>
+      <c r="B241" s="4"/>
+      <c r="C241" s="4"/>
+      <c r="D241" s="5" t="s">
+        <v>2385</v>
+      </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>2925</v>
       </c>
+      <c r="B242" s="4"/>
+      <c r="C242" s="4"/>
+      <c r="D242" s="4"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
@@ -12458,46 +12552,81 @@
       <c r="A244" t="s">
         <v>2979</v>
       </c>
+      <c r="B244" s="4"/>
+      <c r="C244" s="4"/>
+      <c r="D244" s="4"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>2906</v>
       </c>
+      <c r="B245" s="4"/>
+      <c r="C245" s="4"/>
+      <c r="D245" s="4"/>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>2860</v>
       </c>
+      <c r="B246" s="4"/>
+      <c r="C246" s="4"/>
+      <c r="D246" s="4"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>3008</v>
       </c>
+      <c r="B247" s="4"/>
+      <c r="C247" s="4"/>
+      <c r="D247" s="4"/>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>452</v>
       </c>
+      <c r="B248" s="4"/>
+      <c r="C248" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="D248" s="4" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>2985</v>
       </c>
+      <c r="B249" s="4"/>
+      <c r="C249" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="D249" s="5" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>2873</v>
       </c>
+      <c r="B250" s="4"/>
+      <c r="C250" s="4"/>
+      <c r="D250" s="4"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>2823</v>
       </c>
+      <c r="B251" s="4"/>
+      <c r="C251" s="4"/>
+      <c r="D251" s="4"/>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>3035</v>
       </c>
+      <c r="B252" s="4"/>
+      <c r="C252" s="4"/>
+      <c r="D252" s="4"/>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
@@ -12511,53 +12640,99 @@
       <c r="A254" t="s">
         <v>3054</v>
       </c>
+      <c r="B254" s="4"/>
+      <c r="C254" s="4"/>
+      <c r="D254" s="4"/>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>2854</v>
       </c>
+      <c r="B255" s="4"/>
+      <c r="C255" s="4"/>
+      <c r="D255" s="4"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>2853</v>
       </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B256" s="4"/>
+      <c r="C256" s="4"/>
+      <c r="D256" s="4"/>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>2852</v>
       </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B257" s="4"/>
+      <c r="C257" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D257" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>3049</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B258" s="4"/>
+      <c r="C258" s="4"/>
+      <c r="D258" s="4"/>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>2894</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B259" s="4"/>
+      <c r="C259" s="4"/>
+      <c r="D259" s="4"/>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>2893</v>
       </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B260" s="4"/>
+      <c r="C260" s="4"/>
+      <c r="D260" s="4"/>
+      <c r="G260" s="4" t="s">
+        <v>3139</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>2889</v>
       </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B261" s="4"/>
+      <c r="C261" s="5" t="s">
+        <v>3138</v>
+      </c>
+      <c r="D261" s="4" t="s">
+        <v>3139</v>
+      </c>
+      <c r="F261" s="1"/>
+      <c r="G261" s="1" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>2987</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B262" s="4"/>
+      <c r="C262" s="4"/>
+      <c r="D262" s="4"/>
+      <c r="F262" s="1"/>
+      <c r="G262" s="1" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>2976</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>2976</v>
+        <v>3140</v>
       </c>
       <c r="C263" s="5" t="s">
         <v>358</v>
@@ -12565,28 +12740,64 @@
       <c r="D263" s="5" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G263" s="1" t="s">
+        <v>2469</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>3093</v>
       </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B264" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C264" s="4"/>
+      <c r="D264" s="4"/>
+      <c r="G264" s="1" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>3041</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B265" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C265" s="4"/>
+      <c r="D265" s="4"/>
+      <c r="G265" s="1" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B266" s="4"/>
+      <c r="C266" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="D266" s="5" t="s">
+        <v>3141</v>
+      </c>
+      <c r="E266" s="1"/>
+      <c r="G266" s="1" t="s">
+        <v>2366</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>3100</v>
       </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B267" s="4"/>
+      <c r="C267" s="4"/>
+      <c r="D267" s="4"/>
+      <c r="G267" s="1" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>281</v>
       </c>
@@ -12599,104 +12810,231 @@
       <c r="D268" s="4" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G268" s="1" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>2984</v>
       </c>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B269" s="4"/>
+      <c r="C269" s="4"/>
+      <c r="D269" s="4"/>
+      <c r="G269" s="1" t="s">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>2928</v>
       </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B270" s="4"/>
+      <c r="C270" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="D270" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="G270" s="1" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B271" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C271" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="D271" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="G271" s="1" t="s">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>3091</v>
       </c>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B272" s="4"/>
+      <c r="C272" s="4"/>
+      <c r="D272" s="4"/>
+      <c r="G272" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>3044</v>
       </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B273" s="4"/>
+      <c r="C273" s="4"/>
+      <c r="D273" s="4"/>
+      <c r="G273" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>2927</v>
       </c>
       <c r="B274" s="4"/>
       <c r="C274" s="4"/>
       <c r="D274" s="4"/>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G274" s="1" t="s">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>2831</v>
       </c>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B275" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C275" s="4"/>
+      <c r="D275" s="4"/>
+      <c r="G275" s="1" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>2878</v>
       </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B276" s="4"/>
+      <c r="C276" s="4"/>
+      <c r="D276" s="4"/>
+      <c r="G276" s="1" t="s">
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>2887</v>
       </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B277" s="4"/>
+      <c r="C277" s="4"/>
+      <c r="D277" s="4"/>
+      <c r="G277" s="1" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>3019</v>
       </c>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B278" s="4"/>
+      <c r="C278" s="4"/>
+      <c r="D278" s="4"/>
+      <c r="G278" s="1" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>2905</v>
       </c>
       <c r="B279" s="4"/>
       <c r="C279" s="4"/>
       <c r="D279" s="4"/>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G279" s="1" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>2833</v>
       </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B280" s="4"/>
+      <c r="C280" s="4"/>
+      <c r="D280" s="5" t="s">
+        <v>2380</v>
+      </c>
+      <c r="G280" s="1" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>2835</v>
       </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B281" s="4"/>
+      <c r="C281" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="D281" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="G281" s="1" t="s">
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>3058</v>
       </c>
-    </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B282" s="4"/>
+      <c r="C282" s="4"/>
+      <c r="D282" s="4"/>
+      <c r="G282" s="1" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B283" s="4"/>
+      <c r="C283" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="D283" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="G283" s="1" t="s">
+        <v>2479</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>2821</v>
       </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B284" s="4"/>
+      <c r="C284" s="4"/>
+      <c r="D284" s="4"/>
+      <c r="G284" s="1" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>2820</v>
       </c>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B285" s="4"/>
+      <c r="C285" s="4"/>
+      <c r="D285" s="4"/>
+      <c r="G285" s="1" t="s">
+        <v>2481</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>2990</v>
       </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B286" s="4"/>
+      <c r="C286" s="4"/>
+      <c r="D286" s="4"/>
+      <c r="G286" s="1" t="s">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>2926</v>
       </c>
@@ -12709,78 +13047,218 @@
       <c r="D287" s="5" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G287" s="1" t="s">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>3061</v>
       </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B288" s="4"/>
+      <c r="C288" s="4"/>
+      <c r="D288" s="4"/>
+      <c r="G288" s="1" t="s">
+        <v>2485</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>3063</v>
       </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B289" s="4"/>
+      <c r="C289" s="4"/>
+      <c r="D289" s="4"/>
+      <c r="G289" s="1" t="s">
+        <v>2486</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>2861</v>
       </c>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B290" s="4"/>
+      <c r="C290" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D290" s="5" t="s">
+        <v>3142</v>
+      </c>
+      <c r="G290" s="1" t="s">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>2912</v>
       </c>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B291" s="4"/>
+      <c r="C291" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="D291" s="5" t="s">
+        <v>3143</v>
+      </c>
+      <c r="G291" s="1" t="s">
+        <v>2488</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>2943</v>
       </c>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B292" s="4"/>
+      <c r="C292" s="4"/>
+      <c r="D292" s="5" t="s">
+        <v>1907</v>
+      </c>
+      <c r="G292" s="1" t="s">
+        <v>2489</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>3056</v>
       </c>
-    </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B293" s="4"/>
+      <c r="C293" s="4"/>
+      <c r="D293" s="5"/>
+      <c r="E293" s="11" t="s">
+        <v>3145</v>
+      </c>
+      <c r="G293" s="1" t="s">
+        <v>2490</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>2866</v>
       </c>
-    </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B294" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C294" s="5" t="s">
+        <v>3144</v>
+      </c>
+      <c r="D294" s="4" t="s">
+        <v>3145</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G294" s="1" t="s">
+        <v>2491</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>2952</v>
       </c>
-    </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B295" s="4"/>
+      <c r="C295" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="D295" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>2706</v>
+      </c>
+      <c r="G295" s="1" t="s">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>3050</v>
       </c>
-    </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B296" s="4"/>
+      <c r="C296" s="4"/>
+      <c r="D296" s="4"/>
+      <c r="E296" s="1" t="s">
+        <v>2707</v>
+      </c>
+      <c r="G296" s="1" t="s">
+        <v>2493</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>3051</v>
       </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B297" s="4"/>
+      <c r="C297" s="5"/>
+      <c r="D297" s="4"/>
+      <c r="E297" s="1" t="s">
+        <v>2708</v>
+      </c>
+      <c r="G297" s="1" t="s">
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>2819</v>
       </c>
-    </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B298" s="4"/>
+      <c r="C298" s="5"/>
+      <c r="D298" s="4"/>
+      <c r="E298" s="1" t="s">
+        <v>2709</v>
+      </c>
+      <c r="G298" s="1" t="s">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>2882</v>
       </c>
-    </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B299" s="4"/>
+      <c r="C299" s="4"/>
+      <c r="D299" s="4"/>
+      <c r="E299" s="1" t="s">
+        <v>2710</v>
+      </c>
+      <c r="G299" s="1" t="s">
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>3010</v>
       </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B300" s="4"/>
+      <c r="C300" s="4"/>
+      <c r="D300" s="4"/>
+      <c r="E300" s="1" t="s">
+        <v>2704</v>
+      </c>
+      <c r="G300" s="1" t="s">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>2961</v>
       </c>
-    </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B301" s="5" t="s">
+        <v>3146</v>
+      </c>
+      <c r="C301" s="5" t="s">
+        <v>623</v>
+      </c>
+      <c r="D301" s="5" t="s">
+        <v>623</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>2711</v>
+      </c>
+      <c r="G301" s="1" t="s">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>2864</v>
       </c>
@@ -12793,8 +13271,11 @@
       <c r="D302" s="5" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E302" s="1" t="s">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>2865</v>
       </c>
@@ -12807,8 +13288,11 @@
       <c r="D303" s="5" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E303" s="1" t="s">
+        <v>2713</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>2975</v>
       </c>
@@ -12819,46 +13303,72 @@
       <c r="D304" s="4" t="s">
         <v>3117</v>
       </c>
-    </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E304" s="1" t="s">
+        <v>2714</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>3004</v>
       </c>
       <c r="B305" s="4"/>
       <c r="C305" s="4"/>
       <c r="D305" s="4"/>
-    </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E305" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>3103</v>
       </c>
-    </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B306" s="4"/>
+      <c r="C306" s="4"/>
+      <c r="D306" s="4"/>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>3101</v>
       </c>
-    </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B307" s="4"/>
+      <c r="C307" s="4"/>
+      <c r="D307" s="5" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>2857</v>
       </c>
-    </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B308" s="4"/>
+      <c r="C308" s="4"/>
+      <c r="D308" s="5"/>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>2859</v>
       </c>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B309" s="4"/>
+      <c r="C309" s="4"/>
+      <c r="D309" s="4"/>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>2855</v>
       </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B310" s="5"/>
+      <c r="C310" s="4"/>
+      <c r="D310" s="4"/>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>3037</v>
       </c>
-    </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B311" s="4"/>
+      <c r="C311" s="4"/>
+      <c r="D311" s="4"/>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>2916</v>
       </c>
@@ -12868,7 +13378,7 @@
       <c r="C312" s="4"/>
       <c r="D312" s="4"/>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>2917</v>
       </c>
@@ -12876,23 +13386,33 @@
       <c r="C313" s="4"/>
       <c r="D313" s="4"/>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>2918</v>
       </c>
-      <c r="B314" s="1"/>
-    </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B314" s="5"/>
+      <c r="C314" s="4"/>
+      <c r="D314" s="4"/>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>2992</v>
       </c>
-    </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B315" s="4"/>
+      <c r="C315" s="4"/>
+      <c r="D315" s="4"/>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>2922</v>
       </c>
-    </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B316" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C316" s="4"/>
+      <c r="D316" s="4"/>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>2996</v>
       </c>
@@ -12900,7 +13420,7 @@
       <c r="C317" s="4"/>
       <c r="D317" s="4"/>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>449</v>
       </c>
@@ -12914,15 +13434,21 @@
         <v>449</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>2947</v>
       </c>
-    </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B319" s="4"/>
+      <c r="C319" s="4"/>
+      <c r="D319" s="4"/>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>3043</v>
       </c>
+      <c r="B320" s="4"/>
+      <c r="C320" s="4"/>
+      <c r="D320" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A320">
@@ -12937,8 +13463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAB156A-F1D2-EC44-883B-91991D29CBD6}">
   <dimension ref="A1:B273"/>
   <sheetViews>
-    <sheetView topLeftCell="A249" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B262" sqref="B262"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12971,6 +13497,9 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>501</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -13037,6 +13566,9 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2922</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>169</v>
       </c>
@@ -14123,16 +14655,25 @@
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>2976</v>
+      </c>
       <c r="B221" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>3093</v>
+      </c>
       <c r="B222" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>3041</v>
+      </c>
       <c r="B223" s="1" t="s">
         <v>84</v>
       </c>
@@ -14181,6 +14722,9 @@
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>2831</v>
+      </c>
       <c r="B232" s="1" t="s">
         <v>18</v>
       </c>
@@ -14250,6 +14794,9 @@
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>2866</v>
+      </c>
       <c r="B244" s="1" t="s">
         <v>57</v>
       </c>
@@ -14305,11 +14852,17 @@
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>2961</v>
+      </c>
       <c r="B255" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>2961</v>
+      </c>
       <c r="B256" s="1" t="s">
         <v>183</v>
       </c>
@@ -14433,8 +14986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC87240-39B2-2D45-960E-6784B043F1CF}">
   <dimension ref="A1:B436"/>
   <sheetViews>
-    <sheetView topLeftCell="A407" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B421" sqref="B421"/>
+    <sheetView topLeftCell="A353" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B366" sqref="B366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14472,6 +15025,9 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2937</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>376</v>
       </c>
@@ -14637,6 +15193,9 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>2985</v>
+      </c>
       <c r="B36" s="1" t="s">
         <v>556</v>
       </c>
@@ -14706,6 +15265,9 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>2912</v>
+      </c>
       <c r="B48" s="1" t="s">
         <v>416</v>
       </c>
@@ -14765,7 +15327,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>3132</v>
+        <v>3131</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>429</v>
@@ -15754,6 +16316,9 @@
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>2856</v>
+      </c>
       <c r="B239" s="1" t="s">
         <v>626</v>
       </c>
@@ -15764,6 +16329,9 @@
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>2852</v>
+      </c>
       <c r="B241" s="1" t="s">
         <v>318</v>
       </c>
@@ -16036,6 +16604,9 @@
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>2961</v>
+      </c>
       <c r="B290" s="1" t="s">
         <v>623</v>
       </c>
@@ -16090,7 +16661,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>2855</v>
+        <v>2856</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>279</v>
@@ -16205,162 +16776,168 @@
         <v>374</v>
       </c>
     </row>
-    <row r="321" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B321" s="1" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="322" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B322" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="323" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B323" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="324" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B324" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="325" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B325" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B326" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="327" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B327" s="1" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="328" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B328" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="329" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B329" s="1" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="330" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B330" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="331" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B331" s="1" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="332" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B332" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="333" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>2915</v>
+      </c>
       <c r="B333" s="1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="334" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B334" s="1" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="335" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B335" s="1" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="336" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B336" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="337" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B337" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="338" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B338" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="339" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B339" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="340" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B340" s="1" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="341" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B341" s="1" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="342" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B342" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="343" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B343" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="344" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B344" s="1" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="345" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B345" s="1" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="346" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A346" t="s">
+        <v>452</v>
+      </c>
       <c r="B346" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="347" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B347" s="1" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="348" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B348" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="349" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B349" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="350" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B350" s="1" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="351" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B351" s="1" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="352" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B352" s="1" t="s">
         <v>504</v>
       </c>
@@ -16426,11 +17003,17 @@
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A365" t="s">
+        <v>2889</v>
+      </c>
       <c r="B365" s="1" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A366" t="s">
+        <v>2889</v>
+      </c>
       <c r="B366" s="1" t="s">
         <v>451</v>
       </c>
@@ -16454,6 +17037,9 @@
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A370" t="s">
+        <v>680</v>
+      </c>
       <c r="B370" s="1" t="s">
         <v>680</v>
       </c>
@@ -16472,11 +17058,17 @@
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A373" t="s">
+        <v>2928</v>
+      </c>
       <c r="B373" s="1" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A374" t="s">
+        <v>501</v>
+      </c>
       <c r="B374" s="1" t="s">
         <v>501</v>
       </c>
@@ -16565,11 +17157,17 @@
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A391" t="s">
+        <v>2835</v>
+      </c>
       <c r="B391" s="1" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A392" t="s">
+        <v>523</v>
+      </c>
       <c r="B392" s="1" t="s">
         <v>523</v>
       </c>
@@ -16600,6 +17198,9 @@
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A398" t="s">
+        <v>2861</v>
+      </c>
       <c r="B398" s="1" t="s">
         <v>362</v>
       </c>
@@ -16614,82 +17215,91 @@
         <v>701</v>
       </c>
     </row>
-    <row r="401" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B401" s="1" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="402" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B402" s="1" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="403" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A403" t="s">
+        <v>2866</v>
+      </c>
       <c r="B403" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="404" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A404" t="s">
+        <v>2866</v>
+      </c>
       <c r="B404" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="405" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B405" s="1" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="406" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A406" t="s">
+        <v>2952</v>
+      </c>
       <c r="B406" s="1" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="407" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B407" s="1" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="408" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B408" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="409" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B409" s="1" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="410" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B410" s="1" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="411" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B411" s="1" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="412" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B412" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="413" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B413" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="414" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B414" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="415" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B415" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="416" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B416" s="1" t="s">
         <v>537</v>
       </c>
@@ -16705,6 +17315,9 @@
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A419" t="s">
+        <v>2856</v>
+      </c>
       <c r="B419" s="1" t="s">
         <v>277</v>
       </c>
@@ -16813,8 +17426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A27DD5-9C45-4540-ACA5-15A282443161}">
   <dimension ref="A1:B2533"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A1970" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1983" sqref="B1983"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16986,82 +17599,88 @@
         <v>860</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>1861</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>1870</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>1130</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>2523</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>878</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>867</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>2871</v>
+      </c>
       <c r="B44" s="1" t="s">
         <v>2369</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>2937</v>
+      </c>
       <c r="B45" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>612</v>
       </c>
@@ -17294,11 +17913,17 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>2912</v>
+      </c>
       <c r="B92" s="1" t="s">
         <v>2692</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>2912</v>
+      </c>
       <c r="B93" s="1" t="s">
         <v>907</v>
       </c>
@@ -17773,6 +18398,9 @@
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>2985</v>
+      </c>
       <c r="B186" s="1" t="s">
         <v>556</v>
       </c>
@@ -18117,6 +18745,9 @@
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>2912</v>
+      </c>
       <c r="B253" s="1" t="s">
         <v>416</v>
       </c>
@@ -18311,6 +18942,9 @@
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>2889</v>
+      </c>
       <c r="B290" s="1" t="s">
         <v>1038</v>
       </c>
@@ -20373,82 +21007,85 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="657" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="657" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A657" t="s">
+        <v>3101</v>
+      </c>
       <c r="B657" s="1" t="s">
         <v>1365</v>
       </c>
     </row>
-    <row r="658" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="658" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B658" s="1" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="659" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="659" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B659" s="1" t="s">
         <v>2678</v>
       </c>
     </row>
-    <row r="660" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="660" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B660" s="1" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="661" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B661" s="1" t="s">
         <v>1367</v>
       </c>
     </row>
-    <row r="662" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="662" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B662" s="1" t="s">
         <v>1368</v>
       </c>
     </row>
-    <row r="663" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="663" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B663" s="1" t="s">
         <v>1369</v>
       </c>
     </row>
-    <row r="664" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="664" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B664" s="1" t="s">
         <v>2231</v>
       </c>
     </row>
-    <row r="665" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="665" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B665" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="666" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="666" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B666" s="1" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="667" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="667" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B667" s="1" t="s">
         <v>1371</v>
       </c>
     </row>
-    <row r="668" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="668" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B668" s="1" t="s">
         <v>1372</v>
       </c>
     </row>
-    <row r="669" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="669" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B669" s="1" t="s">
         <v>1373</v>
       </c>
     </row>
-    <row r="670" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="670" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B670" s="1" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="671" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="671" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B671" s="1" t="s">
         <v>1375</v>
       </c>
     </row>
-    <row r="672" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="672" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B672" s="1" t="s">
         <v>1346</v>
       </c>
@@ -21148,6 +21785,9 @@
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A798" t="s">
+        <v>2889</v>
+      </c>
       <c r="B798" s="1" t="s">
         <v>1475</v>
       </c>
@@ -22634,6 +23274,9 @@
       </c>
     </row>
     <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1085" t="s">
+        <v>2871</v>
+      </c>
       <c r="B1085" s="1" t="s">
         <v>865</v>
       </c>
@@ -24168,162 +24811,174 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="1377" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1377" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1377" t="s">
+        <v>2852</v>
+      </c>
       <c r="B1377" s="1" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="1378" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1378" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="1379" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1379" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1379" t="s">
+        <v>2852</v>
+      </c>
       <c r="B1379" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="1380" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1380" s="1" t="s">
         <v>1892</v>
       </c>
     </row>
-    <row r="1381" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1381" s="1" t="s">
         <v>1893</v>
       </c>
     </row>
-    <row r="1382" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1382" s="1" t="s">
         <v>1894</v>
       </c>
     </row>
-    <row r="1383" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1383" s="1" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="1384" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1384" s="1" t="s">
         <v>1895</v>
       </c>
     </row>
-    <row r="1385" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1385" s="1" t="s">
         <v>1896</v>
       </c>
     </row>
-    <row r="1386" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1386" s="1" t="s">
         <v>1005</v>
       </c>
     </row>
-    <row r="1387" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1387" s="1" t="s">
         <v>1897</v>
       </c>
     </row>
-    <row r="1388" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1388" s="1" t="s">
         <v>1899</v>
       </c>
     </row>
-    <row r="1389" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1389" s="1" t="s">
         <v>2351</v>
       </c>
     </row>
-    <row r="1390" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1390" s="1" t="s">
         <v>1903</v>
       </c>
     </row>
-    <row r="1391" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1391" s="1" t="s">
         <v>1900</v>
       </c>
     </row>
-    <row r="1392" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1392" s="1" t="s">
         <v>1675</v>
       </c>
     </row>
-    <row r="1393" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1393" s="1" t="s">
         <v>1901</v>
       </c>
     </row>
-    <row r="1394" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1394" s="1" t="s">
         <v>1548</v>
       </c>
     </row>
-    <row r="1395" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1395" s="1" t="s">
         <v>1824</v>
       </c>
     </row>
-    <row r="1396" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1396" s="1" t="s">
         <v>1825</v>
       </c>
     </row>
-    <row r="1397" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1397" s="1" t="s">
         <v>1904</v>
       </c>
     </row>
-    <row r="1398" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1398" s="1" t="s">
         <v>1905</v>
       </c>
     </row>
-    <row r="1399" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1399" s="1" t="s">
         <v>1906</v>
       </c>
     </row>
-    <row r="1400" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1400" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1400" t="s">
+        <v>2943</v>
+      </c>
       <c r="B1400" s="1" t="s">
         <v>1907</v>
       </c>
     </row>
-    <row r="1401" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1401" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1401" t="s">
+        <v>2889</v>
+      </c>
       <c r="B1401" s="1" t="s">
         <v>2469</v>
       </c>
     </row>
-    <row r="1402" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1402" s="1" t="s">
         <v>1908</v>
       </c>
     </row>
-    <row r="1403" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1403" s="1" t="s">
         <v>1337</v>
       </c>
     </row>
-    <row r="1404" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1404" s="1" t="s">
         <v>2105</v>
       </c>
     </row>
-    <row r="1405" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1405" s="1" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="1406" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1406" s="1" t="s">
         <v>1910</v>
       </c>
     </row>
-    <row r="1407" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1407" s="1" t="s">
         <v>1911</v>
       </c>
     </row>
-    <row r="1408" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1408" s="1" t="s">
         <v>1912</v>
       </c>
@@ -24901,6 +25556,9 @@
       </c>
     </row>
     <row r="1516" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1516" t="s">
+        <v>2889</v>
+      </c>
       <c r="B1516" s="1" t="s">
         <v>1985</v>
       </c>
@@ -25872,6 +26530,9 @@
       </c>
     </row>
     <row r="1706" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1706" t="s">
+        <v>2961</v>
+      </c>
       <c r="B1706" s="1" t="s">
         <v>623</v>
       </c>
@@ -26149,7 +26810,7 @@
     </row>
     <row r="1754" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1754" t="s">
-        <v>2855</v>
+        <v>2856</v>
       </c>
       <c r="B1754" s="1" t="s">
         <v>279</v>
@@ -26157,7 +26818,7 @@
     </row>
     <row r="1755" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1755" t="s">
-        <v>2855</v>
+        <v>2856</v>
       </c>
       <c r="B1755" s="1" t="s">
         <v>2206</v>
@@ -26926,82 +27587,85 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="1905" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1905" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1905" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="1906" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1906" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1906" s="1" t="s">
         <v>2326</v>
       </c>
     </row>
-    <row r="1907" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1907" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1907" s="1" t="s">
         <v>2327</v>
       </c>
     </row>
-    <row r="1908" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1908" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1908" s="1" t="s">
         <v>2328</v>
       </c>
     </row>
-    <row r="1909" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1909" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1909" s="1" t="s">
         <v>2329</v>
       </c>
     </row>
-    <row r="1910" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1910" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1910" s="1" t="s">
         <v>2330</v>
       </c>
     </row>
-    <row r="1911" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1911" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1911" s="1" t="s">
         <v>2331</v>
       </c>
     </row>
-    <row r="1912" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1912" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1912" s="1" t="s">
         <v>2333</v>
       </c>
     </row>
-    <row r="1913" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1913" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1913" s="1" t="s">
         <v>2759</v>
       </c>
     </row>
-    <row r="1914" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1914" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1914" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="1915" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1915" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1915" s="1" t="s">
         <v>2334</v>
       </c>
     </row>
-    <row r="1916" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1916" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1916" t="s">
+        <v>2889</v>
+      </c>
       <c r="B1916" s="1" t="s">
         <v>1984</v>
       </c>
     </row>
-    <row r="1917" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1917" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1917" s="1" t="s">
         <v>2336</v>
       </c>
     </row>
-    <row r="1918" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1918" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1918" s="1" t="s">
         <v>2337</v>
       </c>
     </row>
-    <row r="1919" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1919" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1919" s="1" t="s">
         <v>2338</v>
       </c>
     </row>
-    <row r="1920" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1920" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1920" s="1" t="s">
         <v>1694</v>
       </c>
@@ -27166,162 +27830,180 @@
         <v>2365</v>
       </c>
     </row>
-    <row r="1953" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1953" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1953" t="s">
+        <v>2889</v>
+      </c>
       <c r="B1953" s="1" t="s">
         <v>2366</v>
       </c>
     </row>
-    <row r="1954" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1954" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1954" s="1" t="s">
         <v>1271</v>
       </c>
     </row>
-    <row r="1955" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1955" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1955" s="1" t="s">
         <v>2368</v>
       </c>
     </row>
-    <row r="1956" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1956" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1956" s="1" t="s">
         <v>2371</v>
       </c>
     </row>
-    <row r="1957" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1957" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1957" s="1" t="s">
         <v>2372</v>
       </c>
     </row>
-    <row r="1958" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1958" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1958" s="1" t="s">
         <v>2374</v>
       </c>
     </row>
-    <row r="1959" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1959" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1959" s="1" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="1960" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1960" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1960" s="1" t="s">
         <v>2375</v>
       </c>
     </row>
-    <row r="1961" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1961" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1961" s="1" t="s">
         <v>1323</v>
       </c>
     </row>
-    <row r="1962" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1962" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1962" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="1963" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1963" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1963" s="1" t="s">
         <v>2376</v>
       </c>
     </row>
-    <row r="1964" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1964" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1964" s="1" t="s">
         <v>2377</v>
       </c>
     </row>
-    <row r="1965" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1965" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1965" s="1" t="s">
         <v>2378</v>
       </c>
     </row>
-    <row r="1966" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1966" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1966" s="1" t="s">
         <v>2379</v>
       </c>
     </row>
-    <row r="1967" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1967" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1967" t="s">
+        <v>2833</v>
+      </c>
       <c r="B1967" s="1" t="s">
         <v>2380</v>
       </c>
     </row>
-    <row r="1968" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1968" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1968" s="1" t="s">
         <v>1891</v>
       </c>
     </row>
-    <row r="1969" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1969" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1969" s="1" t="s">
         <v>2381</v>
       </c>
     </row>
-    <row r="1970" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1970" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1970" t="s">
+        <v>2951</v>
+      </c>
       <c r="B1970" s="1" t="s">
         <v>2383</v>
       </c>
     </row>
-    <row r="1971" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1971" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1971" t="s">
+        <v>2951</v>
+      </c>
       <c r="B1971" s="1" t="s">
         <v>2382</v>
       </c>
     </row>
-    <row r="1972" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1972" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1972" s="1" t="s">
         <v>2196</v>
       </c>
     </row>
-    <row r="1973" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1973" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1973" s="1" t="s">
         <v>2384</v>
       </c>
     </row>
-    <row r="1974" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1974" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1974" t="s">
+        <v>2915</v>
+      </c>
       <c r="B1974" s="1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="1975" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1975" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1975" t="s">
+        <v>2959</v>
+      </c>
       <c r="B1975" s="1" t="s">
         <v>2385</v>
       </c>
     </row>
-    <row r="1976" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1976" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1976" s="1" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="1977" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1977" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1977" s="1" t="s">
         <v>2386</v>
       </c>
     </row>
-    <row r="1978" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1978" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1978" s="1" t="s">
         <v>2387</v>
       </c>
     </row>
-    <row r="1979" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1979" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1979" s="1" t="s">
         <v>2388</v>
       </c>
     </row>
-    <row r="1980" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1980" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1980" s="1" t="s">
         <v>2389</v>
       </c>
     </row>
-    <row r="1981" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1981" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1981" s="1" t="s">
         <v>2390</v>
       </c>
     </row>
-    <row r="1982" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1982" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1982" s="1" t="s">
         <v>2293</v>
       </c>
     </row>
-    <row r="1983" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1983" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1983" s="1" t="s">
         <v>2391</v>
       </c>
     </row>
-    <row r="1984" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1984" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1984" s="1" t="s">
         <v>2393</v>
       </c>
@@ -27486,82 +28168,85 @@
         <v>493</v>
       </c>
     </row>
-    <row r="2017" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2017" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2017" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="2018" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2018" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2018" s="1" t="s">
         <v>2419</v>
       </c>
     </row>
-    <row r="2019" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2019" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2019" s="1" t="s">
         <v>2416</v>
       </c>
     </row>
-    <row r="2020" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2020" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2020" s="1" t="s">
         <v>2420</v>
       </c>
     </row>
-    <row r="2021" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2021" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2021" s="1" t="s">
         <v>2417</v>
       </c>
     </row>
-    <row r="2022" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2022" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2022" s="1" t="s">
         <v>2418</v>
       </c>
     </row>
-    <row r="2023" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2023" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2023" s="1" t="s">
         <v>2421</v>
       </c>
     </row>
-    <row r="2024" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2024" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2024" s="1" t="s">
         <v>2422</v>
       </c>
     </row>
-    <row r="2025" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2025" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2025" s="1" t="s">
         <v>1426</v>
       </c>
     </row>
-    <row r="2026" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2026" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2026" s="1" t="s">
         <v>2671</v>
       </c>
     </row>
-    <row r="2027" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2027" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2027" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="2028" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2028" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2028" s="1" t="s">
         <v>2370</v>
       </c>
     </row>
-    <row r="2029" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2029" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2029" s="1" t="s">
         <v>2424</v>
       </c>
     </row>
-    <row r="2030" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2030" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2030" s="1" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="2031" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2031" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2031" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2031" s="1" t="s">
         <v>1049</v>
       </c>
     </row>
-    <row r="2032" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2032" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2032" s="1" t="s">
         <v>2254</v>
       </c>
@@ -27667,6 +28352,9 @@
       </c>
     </row>
     <row r="2053" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2053" t="s">
+        <v>452</v>
+      </c>
       <c r="B2053" s="1" t="s">
         <v>452</v>
       </c>
@@ -27889,242 +28577,344 @@
         <v>2462</v>
       </c>
     </row>
-    <row r="2097" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2097" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2097" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="2098" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2098" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2098" s="1" t="s">
         <v>2463</v>
       </c>
     </row>
-    <row r="2099" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2099" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2099" s="1" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="2100" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2100" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="2101" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2101" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="2102" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2102" s="1" t="s">
         <v>2465</v>
       </c>
     </row>
-    <row r="2103" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2103" s="1" t="s">
         <v>2268</v>
       </c>
     </row>
-    <row r="2104" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2104" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2104" s="1" t="s">
         <v>1294</v>
       </c>
     </row>
-    <row r="2105" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2105" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2105" s="1" t="s">
         <v>2466</v>
       </c>
     </row>
-    <row r="2106" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2106" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2106" s="1" t="s">
         <v>2467</v>
       </c>
     </row>
-    <row r="2107" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2107" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2107" s="1" t="s">
         <v>2468</v>
       </c>
     </row>
-    <row r="2108" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2108" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2108" s="1" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="2109" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2109" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2109" s="1" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="2110" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2110" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2110" s="1" t="s">
         <v>2483</v>
       </c>
     </row>
-    <row r="2111" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2111" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2111" s="1" t="s">
         <v>2472</v>
       </c>
     </row>
-    <row r="2112" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2112" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2112" s="1" t="s">
         <v>2473</v>
       </c>
     </row>
-    <row r="2113" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2113" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2113" s="1" t="s">
         <v>2474</v>
       </c>
     </row>
-    <row r="2114" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2114" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2114" s="1" t="s">
         <v>2471</v>
       </c>
     </row>
-    <row r="2115" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2115" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2115" s="1" t="s">
         <v>2475</v>
       </c>
     </row>
-    <row r="2116" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2116" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2116" s="1" t="s">
         <v>2476</v>
       </c>
     </row>
-    <row r="2117" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2117" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2117" s="1" t="s">
         <v>2477</v>
       </c>
     </row>
-    <row r="2118" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2118" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2118" s="1" t="s">
         <v>2478</v>
       </c>
     </row>
-    <row r="2119" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2119" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2119" s="1" t="s">
         <v>2479</v>
       </c>
     </row>
-    <row r="2120" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2120" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2120" s="1" t="s">
         <v>2480</v>
       </c>
     </row>
-    <row r="2121" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2121" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2121" s="1" t="s">
         <v>2481</v>
       </c>
     </row>
-    <row r="2122" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2122" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2122" s="1" t="s">
         <v>2482</v>
       </c>
     </row>
-    <row r="2123" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2123" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2123" s="1" t="s">
         <v>2484</v>
       </c>
     </row>
-    <row r="2124" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2124" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2124" s="1" t="s">
         <v>2485</v>
       </c>
     </row>
-    <row r="2125" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2125" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2125" s="1" t="s">
         <v>2486</v>
       </c>
     </row>
-    <row r="2126" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2126" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2126" s="1" t="s">
         <v>2487</v>
       </c>
     </row>
-    <row r="2127" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2127" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2127" s="1" t="s">
         <v>2488</v>
       </c>
     </row>
-    <row r="2128" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2128" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2128" s="1" t="s">
         <v>2489</v>
       </c>
     </row>
-    <row r="2129" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2129" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2129" s="1" t="s">
         <v>2490</v>
       </c>
     </row>
-    <row r="2130" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2130" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2130" s="1" t="s">
         <v>2491</v>
       </c>
     </row>
-    <row r="2131" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2131" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2131" s="1" t="s">
         <v>2492</v>
       </c>
     </row>
-    <row r="2132" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2132" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2132" s="1" t="s">
         <v>2493</v>
       </c>
     </row>
-    <row r="2133" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2133" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2133" s="1" t="s">
         <v>2494</v>
       </c>
     </row>
-    <row r="2134" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2134" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2134" s="1" t="s">
         <v>2495</v>
       </c>
     </row>
-    <row r="2135" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2135" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2135" s="1" t="s">
         <v>2499</v>
       </c>
     </row>
-    <row r="2136" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2136" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2136" s="1" t="s">
         <v>2500</v>
       </c>
     </row>
-    <row r="2137" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2137" t="s">
+        <v>2889</v>
+      </c>
       <c r="B2137" s="1" t="s">
         <v>2502</v>
       </c>
     </row>
-    <row r="2138" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2138" s="1" t="s">
         <v>2503</v>
       </c>
     </row>
-    <row r="2139" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2139" s="1" t="s">
         <v>2504</v>
       </c>
     </row>
-    <row r="2140" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2140" s="1" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="2141" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2141" s="1" t="s">
         <v>2506</v>
       </c>
     </row>
-    <row r="2142" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2142" s="1" t="s">
         <v>2505</v>
       </c>
     </row>
-    <row r="2143" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2143" s="1" t="s">
         <v>2507</v>
       </c>
     </row>
-    <row r="2144" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2144" s="1" t="s">
         <v>2508</v>
       </c>
@@ -28209,82 +28999,88 @@
         <v>2521</v>
       </c>
     </row>
-    <row r="2161" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2161" s="1" t="s">
         <v>2522</v>
       </c>
     </row>
-    <row r="2162" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2162" s="1" t="s">
         <v>1150</v>
       </c>
     </row>
-    <row r="2163" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2163" s="1" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="2164" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2164" s="1" t="s">
         <v>2525</v>
       </c>
     </row>
-    <row r="2165" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2165" s="1" t="s">
+        <v>680</v>
+      </c>
       <c r="B2165" s="1" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="2166" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2166" s="1" t="s">
+        <v>680</v>
+      </c>
       <c r="B2166" s="1" t="s">
         <v>2526</v>
       </c>
     </row>
-    <row r="2167" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2167" s="1" t="s">
         <v>914</v>
       </c>
     </row>
-    <row r="2168" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2168" s="1" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="2169" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2169" s="1" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="2170" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2170" s="1" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="2171" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2171" s="1" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="2172" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2172" s="1" t="s">
         <v>2527</v>
       </c>
     </row>
-    <row r="2173" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2173" s="1" t="s">
         <v>2528</v>
       </c>
     </row>
-    <row r="2174" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2174" s="1" t="s">
         <v>2529</v>
       </c>
     </row>
-    <row r="2175" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2175" s="1" t="s">
         <v>2530</v>
       </c>
     </row>
-    <row r="2176" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2176" s="1" t="s">
         <v>2531</v>
       </c>
@@ -28323,6 +29119,9 @@
       </c>
     </row>
     <row r="2183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2183" t="s">
+        <v>2928</v>
+      </c>
       <c r="B2183" s="1" t="s">
         <v>415</v>
       </c>
@@ -28333,6 +29132,9 @@
       </c>
     </row>
     <row r="2185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2185" s="1" t="s">
+        <v>501</v>
+      </c>
       <c r="B2185" s="1" t="s">
         <v>501</v>
       </c>
@@ -29015,82 +29817,88 @@
         <v>652</v>
       </c>
     </row>
-    <row r="2321" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2321" s="1" t="s">
         <v>2657</v>
       </c>
     </row>
-    <row r="2322" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2322" s="1" t="s">
         <v>2659</v>
       </c>
     </row>
-    <row r="2323" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2323" s="1" t="s">
         <v>2660</v>
       </c>
     </row>
-    <row r="2324" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2324" s="1" t="s">
         <v>2658</v>
       </c>
     </row>
-    <row r="2325" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2325" s="1" t="s">
         <v>2661</v>
       </c>
     </row>
-    <row r="2326" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2326" s="1" t="s">
         <v>2662</v>
       </c>
     </row>
-    <row r="2327" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2327" t="s">
+        <v>2835</v>
+      </c>
       <c r="B2327" s="1" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="2328" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2328" s="1" t="s">
         <v>2663</v>
       </c>
     </row>
-    <row r="2329" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2329" s="1" t="s">
         <v>2664</v>
       </c>
     </row>
-    <row r="2330" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2330" t="s">
+        <v>523</v>
+      </c>
       <c r="B2330" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="2331" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2331" s="1" t="s">
         <v>2578</v>
       </c>
     </row>
-    <row r="2332" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2332" s="1" t="s">
         <v>2325</v>
       </c>
     </row>
-    <row r="2333" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2333" s="1" t="s">
         <v>2665</v>
       </c>
     </row>
-    <row r="2334" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2334" s="1" t="s">
         <v>2666</v>
       </c>
     </row>
-    <row r="2335" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2335" s="1" t="s">
         <v>2667</v>
       </c>
     </row>
-    <row r="2336" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2336" s="1" t="s">
         <v>2668</v>
       </c>
@@ -29175,322 +29983,367 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="2353" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2353" s="1" t="s">
         <v>2682</v>
       </c>
     </row>
-    <row r="2354" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2354" s="1" t="s">
         <v>1127</v>
       </c>
     </row>
-    <row r="2355" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2355" s="1" t="s">
         <v>2684</v>
       </c>
     </row>
-    <row r="2356" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2356" s="1" t="s">
         <v>2685</v>
       </c>
     </row>
-    <row r="2357" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2357" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="2358" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2358" s="1" t="s">
         <v>2686</v>
       </c>
     </row>
-    <row r="2359" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2359" s="1" t="s">
         <v>2687</v>
       </c>
     </row>
-    <row r="2360" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2360" s="1" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="2361" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2361" s="1" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="2362" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2362" s="1" t="s">
         <v>1682</v>
       </c>
     </row>
-    <row r="2363" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2363" s="1" t="s">
         <v>2688</v>
       </c>
     </row>
-    <row r="2364" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2364" s="1" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="2365" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2365" s="1" t="s">
         <v>2355</v>
       </c>
     </row>
-    <row r="2366" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2366" s="1" t="s">
         <v>1614</v>
       </c>
     </row>
-    <row r="2367" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2367" s="1" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="2368" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2368" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2368" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="B2368" s="1" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="2369" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2369" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2369" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="B2369" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="2370" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2370" s="1" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="2371" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2371" s="1" t="s">
         <v>2690</v>
       </c>
     </row>
-    <row r="2372" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2372" s="1" t="s">
         <v>2691</v>
       </c>
     </row>
-    <row r="2373" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2373" s="1" t="s">
         <v>2693</v>
       </c>
     </row>
-    <row r="2374" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2374" s="1" t="s">
         <v>2694</v>
       </c>
     </row>
-    <row r="2375" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2375" s="1" t="s">
         <v>2695</v>
       </c>
     </row>
-    <row r="2376" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2376" s="1" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="2377" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2377" s="1" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="2378" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2378" s="1" t="s">
         <v>1641</v>
       </c>
     </row>
-    <row r="2379" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2379" s="1" t="s">
         <v>2697</v>
       </c>
     </row>
-    <row r="2380" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2380" s="1" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="2381" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2381" s="1" t="s">
         <v>825</v>
       </c>
     </row>
-    <row r="2382" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2382" s="1" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="2383" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2383" s="1" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="2384" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2384" s="1" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="2385" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2385" s="1" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="2386" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2386" s="1" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="2387" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2387" s="1" t="s">
         <v>2705</v>
       </c>
     </row>
-    <row r="2388" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2388" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2388" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2388" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="2389" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2389" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2389" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2389" s="1" t="s">
         <v>2706</v>
       </c>
     </row>
-    <row r="2390" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2390" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2390" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2390" s="1" t="s">
         <v>2707</v>
       </c>
     </row>
-    <row r="2391" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2391" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2391" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2391" s="1" t="s">
         <v>2708</v>
       </c>
     </row>
-    <row r="2392" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2392" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2392" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2392" s="1" t="s">
         <v>2709</v>
       </c>
     </row>
-    <row r="2393" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2393" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2393" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2393" s="1" t="s">
         <v>2710</v>
       </c>
     </row>
-    <row r="2394" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2394" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2394" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2394" s="1" t="s">
         <v>2704</v>
       </c>
     </row>
-    <row r="2395" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2395" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2395" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2395" s="1" t="s">
         <v>2711</v>
       </c>
     </row>
-    <row r="2396" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2396" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2396" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2396" s="1" t="s">
         <v>2712</v>
       </c>
     </row>
-    <row r="2397" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2397" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2397" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2397" s="1" t="s">
         <v>2713</v>
       </c>
     </row>
-    <row r="2398" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2398" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2398" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2398" s="1" t="s">
         <v>2714</v>
       </c>
     </row>
-    <row r="2399" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2399" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2399" t="s">
+        <v>2866</v>
+      </c>
       <c r="B2399" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="2400" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2400" s="1" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="2401" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2401" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2401" t="s">
+        <v>2952</v>
+      </c>
       <c r="B2401" s="1" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="2402" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2402" s="1" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="2403" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2403" s="1" t="s">
         <v>2715</v>
       </c>
     </row>
-    <row r="2404" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2404" s="1" t="s">
         <v>2464</v>
       </c>
     </row>
-    <row r="2405" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2405" s="1" t="s">
         <v>2716</v>
       </c>
     </row>
-    <row r="2406" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2406" s="1" t="s">
         <v>2717</v>
       </c>
     </row>
-    <row r="2407" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2407" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="2408" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2408" s="1" t="s">
         <v>2654</v>
       </c>
     </row>
-    <row r="2409" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2409" s="1" t="s">
         <v>2718</v>
       </c>
     </row>
-    <row r="2410" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2410" s="1" t="s">
         <v>2719</v>
       </c>
     </row>
-    <row r="2411" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2411" s="1" t="s">
         <v>2720</v>
       </c>
     </row>
-    <row r="2412" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2412" s="1" t="s">
         <v>2721</v>
       </c>
     </row>
-    <row r="2413" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2413" s="1" t="s">
         <v>2722</v>
       </c>
     </row>
-    <row r="2414" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2414" s="1" t="s">
         <v>2723</v>
       </c>
     </row>
-    <row r="2415" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2415" s="1" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="2416" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2416" s="1" t="s">
         <v>508</v>
       </c>
@@ -29575,82 +30428,85 @@
         <v>2734</v>
       </c>
     </row>
-    <row r="2433" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2433" s="1" t="s">
         <v>2106</v>
       </c>
     </row>
-    <row r="2434" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2434" s="1" t="s">
         <v>2737</v>
       </c>
     </row>
-    <row r="2435" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2435" s="1" t="s">
         <v>2738</v>
       </c>
     </row>
-    <row r="2436" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2436" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="2437" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2437" s="1" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="2438" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2438" s="1" t="s">
         <v>2741</v>
       </c>
     </row>
-    <row r="2439" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2439" s="1" t="s">
         <v>1546</v>
       </c>
     </row>
-    <row r="2440" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2440" s="1" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="2441" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2441" s="1" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="2442" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2442" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="2443" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2443" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2443" t="s">
+        <v>2856</v>
+      </c>
       <c r="B2443" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="2444" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2444" s="1" t="s">
         <v>2743</v>
       </c>
     </row>
-    <row r="2445" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2445" s="1" t="s">
         <v>2744</v>
       </c>
     </row>
-    <row r="2446" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2446" s="1" t="s">
         <v>2745</v>
       </c>
     </row>
-    <row r="2447" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2447" s="1" t="s">
         <v>2746</v>
       </c>
     </row>
-    <row r="2448" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2448" s="1" t="s">
         <v>2747</v>
       </c>

</xml_diff>